<commit_message>
Updated Master data excels
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-machine_master.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-machine_master.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Desktop\Updated Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8ADB870C-C56A-4DBE-BA01-809B97AB7BCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master-machine_master" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -54,9 +55,6 @@
     <t>Machine 1</t>
   </si>
   <si>
-    <t>e1:01:2b:c2:1d:b0</t>
-  </si>
-  <si>
     <t>NM5328114630</t>
   </si>
   <si>
@@ -298,12 +296,15 @@
   </si>
   <si>
     <t>192.168.0.215</t>
+  </si>
+  <si>
+    <t>8c:16:45:5a:5d:0d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1137,11 +1138,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1192,28 +1193,28 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2">
         <v>1001</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1221,31 +1222,31 @@
         <v>10002</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3">
         <v>1001</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1253,31 +1254,31 @@
         <v>10003</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4">
         <v>1001</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1285,31 +1286,31 @@
         <v>10004</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5">
         <v>1001</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1317,31 +1318,31 @@
         <v>10005</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6">
         <v>1001</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1349,31 +1350,31 @@
         <v>10006</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7">
         <v>1001</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1381,31 +1382,31 @@
         <v>10007</v>
       </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8">
         <v>1001</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1413,31 +1414,31 @@
         <v>10008</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9">
         <v>1001</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1445,31 +1446,31 @@
         <v>10009</v>
       </c>
       <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10">
         <v>1001</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1477,31 +1478,31 @@
         <v>10010</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11">
         <v>1001</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1509,31 +1510,31 @@
         <v>10011</v>
       </c>
       <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12">
         <v>1001</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1541,31 +1542,31 @@
         <v>10012</v>
       </c>
       <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13">
         <v>1001</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1573,31 +1574,31 @@
         <v>10013</v>
       </c>
       <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14">
         <v>1001</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1605,31 +1606,31 @@
         <v>10014</v>
       </c>
       <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15">
         <v>1001</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1637,31 +1638,31 @@
         <v>10015</v>
       </c>
       <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16">
         <v>1001</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1669,31 +1670,31 @@
         <v>10016</v>
       </c>
       <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="D17" t="s">
-        <v>60</v>
-      </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F17">
         <v>1001</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1701,31 +1702,31 @@
         <v>10017</v>
       </c>
       <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18">
         <v>1001</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1733,31 +1734,31 @@
         <v>10018</v>
       </c>
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>65</v>
       </c>
-      <c r="D19" t="s">
-        <v>66</v>
-      </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F19">
         <v>1001</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1765,31 +1766,31 @@
         <v>10019</v>
       </c>
       <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20">
         <v>1001</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1797,35 +1798,35 @@
         <v>10020</v>
       </c>
       <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21">
         <v>1001</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Master Dara excels
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-machine_master.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-machine_master.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8ADB870C-C56A-4DBE-BA01-809B97AB7BCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2B3FB1BF-5524-4865-9DF6-6EB6668CAAFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -70,171 +70,114 @@
     <t>Machine 2</t>
   </si>
   <si>
-    <t>e9:0e:a3:05:d5:8d</t>
-  </si>
-  <si>
     <t>WY2132605316</t>
   </si>
   <si>
     <t>Machine 3</t>
   </si>
   <si>
-    <t>f9:87:3f:16:65:92</t>
-  </si>
-  <si>
     <t>CM6384145127</t>
   </si>
   <si>
     <t>Machine 4</t>
   </si>
   <si>
-    <t>cc:11:b1:fd:1b:a6</t>
-  </si>
-  <si>
     <t>NT894252578</t>
   </si>
   <si>
     <t>Machine 5</t>
   </si>
   <si>
-    <t>bf:91:79:24:23:85</t>
-  </si>
-  <si>
     <t>YM866672706</t>
   </si>
   <si>
     <t>Machine 6</t>
   </si>
   <si>
-    <t>6e:ee:fe:f7:50:24</t>
-  </si>
-  <si>
     <t>WT6501645780</t>
   </si>
   <si>
     <t>Machine 7</t>
   </si>
   <si>
-    <t>6d:a6:30:56:66:9f</t>
-  </si>
-  <si>
     <t>LK8186452621</t>
   </si>
   <si>
     <t>Machine 8</t>
   </si>
   <si>
-    <t>2b:9f:5c:a1:d6:d3</t>
-  </si>
-  <si>
     <t>NR3264783870</t>
   </si>
   <si>
     <t>Machine 9</t>
   </si>
   <si>
-    <t>ee:9e:95:a6:cb:14</t>
-  </si>
-  <si>
     <t>RW437027336</t>
   </si>
   <si>
     <t>Machine 10</t>
   </si>
   <si>
-    <t>17:dd:46:75:ae:0d</t>
-  </si>
-  <si>
     <t>SI158158531</t>
   </si>
   <si>
     <t>Machine 11</t>
   </si>
   <si>
-    <t>26:e0:5a:44:b4:f2</t>
-  </si>
-  <si>
     <t>XF3416823469</t>
   </si>
   <si>
     <t>Machine 12</t>
   </si>
   <si>
-    <t>1f:ce:cf:7a:e4:c8</t>
-  </si>
-  <si>
     <t>BW4524978011</t>
   </si>
   <si>
     <t>Machine 13</t>
   </si>
   <si>
-    <t>c8:5f:95:d9:16:d0</t>
-  </si>
-  <si>
     <t>DB289579153</t>
   </si>
   <si>
     <t>Machine 14</t>
   </si>
   <si>
-    <t>e0:be:be:a8:77:10</t>
-  </si>
-  <si>
     <t>SI4597903231</t>
   </si>
   <si>
     <t>Machine 15</t>
   </si>
   <si>
-    <t>12:80:c6:7c:95:d3</t>
-  </si>
-  <si>
     <t>TJ7809002958</t>
   </si>
   <si>
     <t>Machine 16</t>
   </si>
   <si>
-    <t>43:71:17:27:9b:65</t>
-  </si>
-  <si>
     <t>JR6082789079</t>
   </si>
   <si>
     <t>Machine 17</t>
   </si>
   <si>
-    <t>c2:f2:53:92:df:04</t>
-  </si>
-  <si>
     <t>SA3722889241</t>
   </si>
   <si>
     <t>Machine 18</t>
   </si>
   <si>
-    <t>bf:8e:1d:4e:75:00</t>
-  </si>
-  <si>
     <t>RR2683722548</t>
   </si>
   <si>
     <t>Machine 19</t>
   </si>
   <si>
-    <t>36:bf:1e:3a:2d:b0</t>
-  </si>
-  <si>
     <t>PO6528391346</t>
   </si>
   <si>
     <t>Machine 20</t>
   </si>
   <si>
-    <t>21:43:ab:46:59:21</t>
-  </si>
-  <si>
     <t>FB5962911652</t>
   </si>
   <si>
@@ -298,7 +241,172 @@
     <t>192.168.0.215</t>
   </si>
   <si>
-    <t>8c:16:45:5a:5d:0d</t>
+    <t>FB5962911653</t>
+  </si>
+  <si>
+    <t>FB5962911654</t>
+  </si>
+  <si>
+    <t>FB5962911655</t>
+  </si>
+  <si>
+    <t>FB5962911656</t>
+  </si>
+  <si>
+    <t>FB5962911657</t>
+  </si>
+  <si>
+    <t>FB5962911658</t>
+  </si>
+  <si>
+    <t>FB5962911659</t>
+  </si>
+  <si>
+    <t>FB5962911661</t>
+  </si>
+  <si>
+    <t>FB5962911662</t>
+  </si>
+  <si>
+    <t>192.168.0.874</t>
+  </si>
+  <si>
+    <t>192.168.0.721</t>
+  </si>
+  <si>
+    <t>192.168.0.841</t>
+  </si>
+  <si>
+    <t>192.168.0.186</t>
+  </si>
+  <si>
+    <t>192.168.0.627</t>
+  </si>
+  <si>
+    <t>192.168.0.879</t>
+  </si>
+  <si>
+    <t>192.168.0.628</t>
+  </si>
+  <si>
+    <t>192.168.0.306</t>
+  </si>
+  <si>
+    <t>192.168.0.355</t>
+  </si>
+  <si>
+    <t>Machine 21</t>
+  </si>
+  <si>
+    <t>Machine 22</t>
+  </si>
+  <si>
+    <t>Machine 23</t>
+  </si>
+  <si>
+    <t>Machine 24</t>
+  </si>
+  <si>
+    <t>Machine 25</t>
+  </si>
+  <si>
+    <t>Machine 26</t>
+  </si>
+  <si>
+    <t>Machine 27</t>
+  </si>
+  <si>
+    <t>Machine 28</t>
+  </si>
+  <si>
+    <t>Machine 29</t>
+  </si>
+  <si>
+    <t>8C-16-45-5A-5D-0D</t>
+  </si>
+  <si>
+    <t>8C-16-45-88-E1-0D</t>
+  </si>
+  <si>
+    <t>00-FF-D3-E3-9A-27</t>
+  </si>
+  <si>
+    <t>8C-16-45-5A-62-41</t>
+  </si>
+  <si>
+    <t>E8-6A-64-1D-75-E4</t>
+  </si>
+  <si>
+    <t>8C-16-45-FA-94-B7</t>
+  </si>
+  <si>
+    <t>8C-16-45-1A-0F-62</t>
+  </si>
+  <si>
+    <t>E8-6A-64-1C-52-6E</t>
+  </si>
+  <si>
+    <t>48-51-B7-10-35-A6</t>
+  </si>
+  <si>
+    <t>8C-16-45-38-F3-F3</t>
+  </si>
+  <si>
+    <t>D4-3D-7E-58-CC-45</t>
+  </si>
+  <si>
+    <t>8C-16-45-5A-5D-96</t>
+  </si>
+  <si>
+    <t>8C-16-45-5A-5D-8E</t>
+  </si>
+  <si>
+    <t>8C-16-45-33-A5-5F</t>
+  </si>
+  <si>
+    <t>3C-95-09-F9-EA-DF</t>
+  </si>
+  <si>
+    <t>8C-16-45-88-E7-0B</t>
+  </si>
+  <si>
+    <t>B4-69-21-5A-DB-C4</t>
+  </si>
+  <si>
+    <t>E8-6A-64-1D-48-B7</t>
+  </si>
+  <si>
+    <t>8C-16-45-59-69-09 </t>
+  </si>
+  <si>
+    <t>98-E7-F4-30-16-5A </t>
+  </si>
+  <si>
+    <t>38-BA-F8-53-C7-8F</t>
+  </si>
+  <si>
+    <t>E8-6A-64-1C-58-C2</t>
+  </si>
+  <si>
+    <t>E4-A4-71-CE-BA-93</t>
+  </si>
+  <si>
+    <t>54-E1-AD-EA-30-C9</t>
+  </si>
+  <si>
+    <t>8C-16-45-65-DD-40</t>
+  </si>
+  <si>
+    <t>58-20-B1-D6-C3-BE</t>
+  </si>
+  <si>
+    <t>8C-16-45-38-F0-25</t>
+  </si>
+  <si>
+    <t>6C-88-14-AC-EF-55</t>
+  </si>
+  <si>
+    <t>3C-6A-A7-C0-DF-27</t>
   </si>
 </sst>
 </file>
@@ -1139,16 +1247,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A31" sqref="A31:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1193,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="F2">
         <v>1001</v>
@@ -1225,13 +1333,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>1001</v>
@@ -1254,16 +1362,16 @@
         <v>10003</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>1001</v>
@@ -1286,16 +1394,16 @@
         <v>10004</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="F5">
         <v>1001</v>
@@ -1318,16 +1426,16 @@
         <v>10005</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="F6">
         <v>1001</v>
@@ -1350,16 +1458,16 @@
         <v>10006</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="F7">
         <v>1001</v>
@@ -1382,16 +1490,16 @@
         <v>10007</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="F8">
         <v>1001</v>
@@ -1414,16 +1522,16 @@
         <v>10008</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="F9">
         <v>1001</v>
@@ -1446,16 +1554,16 @@
         <v>10009</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="F10">
         <v>1001</v>
@@ -1478,16 +1586,16 @@
         <v>10010</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F11">
         <v>1001</v>
@@ -1510,16 +1618,16 @@
         <v>10011</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F12">
         <v>1001</v>
@@ -1542,16 +1650,16 @@
         <v>10012</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="F13">
         <v>1001</v>
@@ -1574,16 +1682,16 @@
         <v>10013</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="F14">
         <v>1001</v>
@@ -1606,16 +1714,16 @@
         <v>10014</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="F15">
         <v>1001</v>
@@ -1638,16 +1746,16 @@
         <v>10015</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="F16">
         <v>1001</v>
@@ -1670,16 +1778,16 @@
         <v>10016</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F17">
         <v>1001</v>
@@ -1702,16 +1810,16 @@
         <v>10017</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="F18">
         <v>1001</v>
@@ -1734,16 +1842,16 @@
         <v>10018</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="F19">
         <v>1001</v>
@@ -1766,16 +1874,16 @@
         <v>10019</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="F20">
         <v>1001</v>
@@ -1798,30 +1906,318 @@
         <v>10020</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21">
+        <v>1001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>10021</v>
+      </c>
+      <c r="B22" t="s">
         <v>91</v>
       </c>
-      <c r="F21">
-        <v>1001</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22">
+        <v>1001</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>10022</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23">
+        <v>1001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>10023</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24">
+        <v>1001</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>10024</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25">
+        <v>1001</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>10025</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26">
+        <v>1001</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>10026</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27">
+        <v>1001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>10027</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28">
+        <v>1001</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>10028</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29">
+        <v>1001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>10029</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30">
+        <v>1001</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>